<commit_message>
add readmes and cleaning script
</commit_message>
<xml_diff>
--- a/Assignment2/data/variables.xlsx
+++ b/Assignment2/data/variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceuedu-my.sharepoint.com/personal/gulacsy_dominik_student_ceu_edu/Documents/1st_trimester/DA2/Assignment1/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceuedu-my.sharepoint.com/personal/gulacsy_dominik_student_ceu_edu/Documents/1st_trimester/DA2/DA2_Assignments/Assignment2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="14_{ED97C292-79C0-4DEA-9D57-E57142A5F012}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D22894E4-3894-468E-81DF-5A9FBBFB0248}"/>
+  <xr:revisionPtr revIDLastSave="188" documentId="14_{ED97C292-79C0-4DEA-9D57-E57142A5F012}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8D93F189-179C-453E-8178-1B1F920C6A47}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>variable</t>
   </si>
@@ -51,21 +51,6 @@
     <t>country</t>
   </si>
   <si>
-    <t>confirmed</t>
-  </si>
-  <si>
-    <t>death</t>
-  </si>
-  <si>
-    <t>recovered</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>population</t>
-  </si>
-  <si>
     <t>quantitative, ratio</t>
   </si>
   <si>
@@ -75,41 +60,104 @@
     <t>unit_of_measurement</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>person</t>
-  </si>
-  <si>
-    <t>the specific country to which COVID metrics and population data belongs</t>
-  </si>
-  <si>
-    <t>the number of persons confirmed and probable to be deceased at least partly due to COVID-19 (where reported)</t>
-  </si>
-  <si>
-    <t>case</t>
-  </si>
-  <si>
-    <t>the number of COVID-19 infection cases confirmed and probable  (where reported)</t>
-  </si>
-  <si>
-    <t>the number of COVID-19 infection cases that ended with recovery, these are estimates based on local media reports, and state and local reporting when available, and therefore may be substantially lower than the true number (where reported)</t>
-  </si>
-  <si>
-    <t>the number of COVID-19 infection cases that are still active, calculated as (total cases - total recovered - total deaths)</t>
-  </si>
-  <si>
-    <t>the population data of the country for 2019</t>
-  </si>
-  <si>
-    <t>Austria</t>
+    <t>iso2c</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>inflation</t>
+  </si>
+  <si>
+    <t>unemployment</t>
+  </si>
+  <si>
+    <t>savings</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>gdpgrowth</t>
+  </si>
+  <si>
+    <t>govexp</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>quantitative, interval</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>General government final consumption expenditure (% of GDP)</t>
+  </si>
+  <si>
+    <t>% (annual)</t>
+  </si>
+  <si>
+    <t>% of total labor force</t>
+  </si>
+  <si>
+    <t>% of GDP</t>
+  </si>
+  <si>
+    <t>GDP growth</t>
+  </si>
+  <si>
+    <t>Broad money</t>
+  </si>
+  <si>
+    <t>Gross savings</t>
+  </si>
+  <si>
+    <t>Unemployment, total (modeled ILO estimate)</t>
+  </si>
+  <si>
+    <t>Inflation, GDP deflator</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Inflation as measured by the annual growth rate of the GDP implicit deflator shows the rate of price change in the economy as a whole. The GDP implicit deflator is the ratio of GDP in current local currency to GDP in constant local currency.</t>
+  </si>
+  <si>
+    <t>Gross savings are calculated as gross national income less total consumption, plus net transfers.</t>
+  </si>
+  <si>
+    <t>Broad money (IFS line 35L..ZK) is the sum of currency outside banks; demand deposits other than those of the central government; the time, savings, and foreign currency deposits of resident sectors other than the central government; bank and traveler’s checks; and other securities such as certificates of deposit and commercial paper.</t>
+  </si>
+  <si>
+    <t>Annual percentage growth rate of GDP at market prices based on constant local currency. Aggregates are based on constant 2010 U.S. dollars. GDP is the sum of gross value added by all resident producers in the economy plus any product taxes and minus any subsidies not included in the value of the products. It is calculated without making deductions for depreciation of fabricated assets or for depletion and degradation of natural resources.</t>
+  </si>
+  <si>
+    <t>General government final consumption expenditure (formerly general government consumption) includes all government current expenditures for purchases of goods and services (including compensation of employees). It also includes most expenditures on national defense and security, but excludes government military expenditures that are part of government capital formation.</t>
+  </si>
+  <si>
+    <t>Unique 2-letter country identifier code</t>
+  </si>
+  <si>
+    <t>The specific country to which economic indicators belong to</t>
+  </si>
+  <si>
+    <t>The year to which economic indicators belong to</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +172,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -173,10 +229,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -184,31 +241,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -486,175 +535,280 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:F7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="64.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="64.85546875" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1.16322395805075</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="5">
+        <v>11.208000183105501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="5">
+        <v>25.323977114693601</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="B8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="5">
+        <v>71.020752535777206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="5">
+        <v>3.4392173522866498</v>
+      </c>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="8">
-        <v>31827</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="8">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="10">
-        <v>26257</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="8">
-        <v>4820</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="8">
-        <v>8877067</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
+      <c r="E10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="5">
+        <v>19.4822769291101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" display="https://data.worldbank.org/indicator/NY.GNS.ICTR.ZS" xr:uid="{B0032C61-DF7D-4D0B-A25D-7CD69AE5B6B7}"/>
+    <hyperlink ref="B8" r:id="rId2" display="https://data.worldbank.org/indicator/FM.LBL.BMNY.GD.ZS" xr:uid="{CF7F0F6A-3EA9-4510-B895-5E8CB1AEC8F6}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://data.worldbank.org/indicator/NY.GDP.DEFL.KD.ZG" xr:uid="{7A327EE4-27C2-4E98-AFBE-8E20876C9D2A}"/>
+    <hyperlink ref="B10" r:id="rId4" xr:uid="{BB0FA81A-60F4-401F-BDEC-C9D83FBB8B9F}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{636C260C-ED4B-4373-9370-34F43B1769FB}"/>
+    <hyperlink ref="B6" r:id="rId6" display="https://data.worldbank.org/indicator/SL.UEM.TOTL.ZS" xr:uid="{A3B7658C-126D-4753-8F7F-AA06BF9E75DC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
carry out data analysis
</commit_message>
<xml_diff>
--- a/Assignment2/data/variables.xlsx
+++ b/Assignment2/data/variables.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceuedu-my.sharepoint.com/personal/gulacsy_dominik_student_ceu_edu/Documents/1st_trimester/DA2/DA2_Assignments/Assignment2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="14_{ED97C292-79C0-4DEA-9D57-E57142A5F012}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E6BAD1BE-2C48-4FE9-86B4-5B245A21E681}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="14_{ED97C292-79C0-4DEA-9D57-E57142A5F012}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F91F9B62-FDAA-4D7B-9C31-FFA81F72CAF5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="var_explanation" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -549,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>